<commit_message>
Added '> ' to loops/prime_numbers.xlsx to preserve spacing.
</commit_message>
<xml_diff>
--- a/loops/prime_numbers.xlsx
+++ b/loops/prime_numbers.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
-    <t>primes = []</t>
+    <t>&gt; primes = []</t>
   </si>
   <si>
     <t>line no.</t>
@@ -32,13 +32,13 @@
     <t>b</t>
   </si>
   <si>
-    <t>for a in range(2, 30):</t>
+    <t>&gt;     for a in range(2, 30):</t>
   </si>
   <si>
     <t>[]</t>
   </si>
   <si>
-    <t>    for b in range(2, a):</t>
+    <t>&gt;         for b in range(2, a):</t>
   </si>
   <si>
     <t>range(2, 30)</t>
@@ -47,25 +47,25 @@
     <t>[2, 3, 4, …, 29]</t>
   </si>
   <si>
-    <t>         if a % b == 0:</t>
+    <t>&gt;             if a % b == 0:</t>
   </si>
   <si>
     <t>range(2, 2)</t>
   </si>
   <si>
-    <t>            break</t>
-  </si>
-  <si>
-    <t>    else:</t>
+    <t>&gt;                 break</t>
+  </si>
+  <si>
+    <t>&gt;     else:</t>
   </si>
   <si>
     <t>[2]</t>
   </si>
   <si>
-    <t>        primes.append(a)</t>
-  </si>
-  <si>
-    <t>print primes</t>
+    <t>&gt;         primes.append(a)</t>
+  </si>
+  <si>
+    <t>&gt; print primes</t>
   </si>
   <si>
     <t>range(2, 3)</t>
@@ -96,15 +96,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -125,6 +125,7 @@
       <sz val="10"/>
       <name val="Liberation Mono;Cumberland AMT;Cumberland;Courier New;Cousine;Nimbus Mono L;DejaVu Sans Mono;Courier;Lucida Sans Typewriter;Lucida Typewriter;Monaco;Monospaced"/>
       <family val="3"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -175,7 +176,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -186,10 +187,6 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -212,7 +209,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -372,7 +369,8 @@
       <c r="H9" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="I9" s="3" t="b">
+      <c r="I9" s="0" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -426,7 +424,8 @@
       <c r="H15" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="I15" s="3" t="b">
+      <c r="I15" s="0" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
@@ -464,7 +463,8 @@
       <c r="H19" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="I19" s="3" t="b">
+      <c r="I19" s="0" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -483,7 +483,8 @@
       <c r="H21" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="I21" s="3" t="b">
+      <c r="I21" s="0" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -502,7 +503,8 @@
       <c r="H23" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="I23" s="3" t="b">
+      <c r="I23" s="0" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>